<commit_message>
Updat data no 8
</commit_message>
<xml_diff>
--- a/data training 65.xlsx
+++ b/data training 65.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dataq\kuliah\Laporan KP\Proposal TA\Data warga miskin krapyak\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AGUS-PC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32EA1AE-4E0B-4009-AFF3-B609ECC0DB5E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4DDAA0-A311-471A-B732-E8DCEE923CAF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{C4810B73-25D7-4A38-B18B-231651BDA47D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="264">
   <si>
     <t>1</t>
   </si>
@@ -821,6 +821,12 @@
   </si>
   <si>
     <t>REKNO</t>
+  </si>
+  <si>
+    <t>KRESNA DEWANTA</t>
+  </si>
+  <si>
+    <t>JL SUGRIWO RT 5 RW 3</t>
   </si>
 </sst>
 </file>
@@ -883,7 +889,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1065,11 +1071,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1106,6 +1125,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1115,11 +1139,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1537,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D731671-C4D2-4EDD-AA27-6FE0F800ED7A}">
   <dimension ref="A1:P114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,41 +1585,41 @@
     <row r="1" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
       <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
       <c r="P2" s="11"/>
     </row>
     <row r="3" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
@@ -1969,37 +1989,37 @@
         <v>7</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>81</v>
+        <v>262</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>82</v>
+        <v>263</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>67</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
+      </c>
+      <c r="L13" s="32" t="s">
+        <v>53</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="N13" s="9"/>
     </row>
@@ -4836,40 +4856,40 @@
       </c>
     </row>
     <row r="85" spans="2:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="27" t="s">
+      <c r="B85" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="C85" s="29" t="s">
+      <c r="C85" s="26" t="s">
         <v>261</v>
       </c>
-      <c r="D85" s="29" t="s">
+      <c r="D85" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="E85" s="29" t="s">
+      <c r="E85" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="F85" s="29" t="s">
+      <c r="F85" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="G85" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="H85" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="I85" s="29" t="s">
+      <c r="G85" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="H85" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="I85" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="J85" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="K85" s="29" t="s">
+      <c r="J85" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="K85" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="L85" s="29" t="s">
+      <c r="L85" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="M85" s="30" t="s">
+      <c r="M85" s="27" t="s">
         <v>70</v>
       </c>
       <c r="N85" s="21"/>
@@ -4881,41 +4901,41 @@
       <c r="N93" s="16"/>
     </row>
     <row r="98" spans="11:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="K98" s="25" t="s">
+      <c r="K98" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="L98" s="25"/>
-      <c r="M98" s="25"/>
+      <c r="L98" s="30"/>
+      <c r="M98" s="30"/>
     </row>
     <row r="99" spans="11:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="K99" s="25" t="s">
+      <c r="K99" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="L99" s="25"/>
-      <c r="M99" s="25"/>
+      <c r="L99" s="30"/>
+      <c r="M99" s="30"/>
     </row>
     <row r="107" spans="11:13" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="K107" s="24" t="s">
+      <c r="K107" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="L107" s="24"/>
-      <c r="M107" s="24"/>
+      <c r="L107" s="29"/>
+      <c r="M107" s="29"/>
     </row>
     <row r="108" spans="11:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="K108" s="25" t="s">
+      <c r="K108" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="L108" s="25"/>
-      <c r="M108" s="25"/>
+      <c r="L108" s="30"/>
+      <c r="M108" s="30"/>
     </row>
     <row r="114" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B114">
         <v>1</v>
       </c>
-      <c r="C114" s="28" t="s">
+      <c r="C114" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="D114" s="28" t="s">
+      <c r="D114" s="25" t="s">
         <v>132</v>
       </c>
       <c r="E114" s="6" t="s">
@@ -4942,7 +4962,7 @@
       <c r="L114" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="M114" s="31" t="s">
+      <c r="M114" s="28" t="s">
         <v>260</v>
       </c>
     </row>

</xml_diff>